<commit_message>
update with the most recent records
</commit_message>
<xml_diff>
--- a/data/opyn-squeeth-20240108215345156.xlsx
+++ b/data/opyn-squeeth-20240108215345156.xlsx
@@ -95,7 +95,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -161,1190 +161,1248 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>1.7044704E12</v>
+        <v>1.7046432E12</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>1.704556799999E12</v>
+        <v>1.704729599999E12</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>1.7044704E12</v>
+        <v>1.70471688E12</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>1.70449602E12</v>
+        <v>1.70465358E12</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>134.608124449251</v>
+        <v>127.50138298269286</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>134.608124449251</v>
+        <v>142.65460279484728</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>129.0846725577171</v>
+        <v>124.31434715670169</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>130.17907193279171</v>
+        <v>139.60983215668782</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>35485.13</v>
+        <v>226599.24</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>1.704384E12</v>
+        <v>1.7045568E12</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>1.704470399999E12</v>
+        <v>1.704643199999E12</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>1.70440098E12</v>
+        <v>1.7046117E12</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>1.70443704E12</v>
+        <v>1.70463798E12</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>133.3822195363162</v>
+        <v>130.17907193279171</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>137.3243900874036</v>
+        <v>132.90844260772263</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>129.55092145959182</v>
+        <v>127.50138298269286</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>134.608124449251</v>
+        <v>127.50138298269286</v>
       </c>
       <c r="I3" s="2" t="n">
-        <v>343826.59</v>
+        <v>104174.43</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>1.7042976E12</v>
+        <v>1.7044704E12</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>1.704383999999E12</v>
+        <v>1.704556799999E12</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>1.70437416E12</v>
+        <v>1.7044704E12</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>1.7042976E12</v>
+        <v>1.70449602E12</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>126.08099515605464</v>
+        <v>134.608124449251</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>133.3822195363162</v>
+        <v>134.608124449251</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>126.08099515605464</v>
+        <v>129.0846725577171</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>133.3822195363162</v>
+        <v>130.17907193279171</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>14036.2</v>
+        <v>35485.13</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>1.7042112E12</v>
+        <v>1.704384E12</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>1.704297599999E12</v>
+        <v>1.704470399999E12</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>1.70421918E12</v>
+        <v>1.70440098E12</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>1.7042562E12</v>
+        <v>1.70443704E12</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>142.21934833917476</v>
+        <v>133.3822195363162</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>143.72345206785002</v>
+        <v>137.3243900874036</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>120.89401488978949</v>
+        <v>129.55092145959182</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>126.08099515605464</v>
+        <v>134.608124449251</v>
       </c>
       <c r="I5" s="2" t="n">
-        <v>190482.02</v>
+        <v>343826.59</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>1.7041248E12</v>
+        <v>1.7042976E12</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>1.704211199999E12</v>
+        <v>1.704383999999E12</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>1.70415726E12</v>
+        <v>1.70437416E12</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>1.70420094E12</v>
+        <v>1.7042976E12</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>143.97540938716227</v>
+        <v>126.08099515605464</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>150.8232388936242</v>
+        <v>133.3822195363162</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>141.9894865288733</v>
+        <v>126.08099515605464</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>142.20173060228947</v>
+        <v>133.3822195363162</v>
       </c>
       <c r="I6" s="2" t="n">
-        <v>60125.93</v>
+        <v>14036.2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>1.7040384E12</v>
+        <v>1.7042112E12</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>1.704124799999E12</v>
+        <v>1.704297599999E12</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>1.70409714E12</v>
+        <v>1.70421918E12</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>1.70405208E12</v>
+        <v>1.7042562E12</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>139.7205451802579</v>
+        <v>142.21934833917476</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>144.5345377228569</v>
+        <v>143.72345206785002</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>139.1579271155912</v>
+        <v>120.89401488978949</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>143.923765948135</v>
+        <v>126.08099515605464</v>
       </c>
       <c r="I7" s="2" t="n">
-        <v>242371.99</v>
+        <v>190482.02</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>1.703952E12</v>
+        <v>1.7041248E12</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>1.704038399999E12</v>
+        <v>1.704211199999E12</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>1.70399796E12</v>
+        <v>1.70415726E12</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>1.703964E12</v>
+        <v>1.70420094E12</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>138.48865502640658</v>
+        <v>143.97540938716227</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>140.63047373957855</v>
+        <v>150.8232388936242</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>137.5574753447999</v>
+        <v>141.9894865288733</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>139.7205451802579</v>
+        <v>142.20173060228947</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>8432.36</v>
+        <v>60125.93</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>1.7038656E12</v>
+        <v>1.7040384E12</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>1.703951999999E12</v>
+        <v>1.704124799999E12</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>1.7038692E12</v>
+        <v>1.70409714E12</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>1.70390106E12</v>
+        <v>1.70405208E12</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>139.7096543691948</v>
+        <v>139.7205451802579</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>140.1036556808429</v>
+        <v>144.5345377228569</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>137.2288543735375</v>
+        <v>139.1579271155912</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>138.48865502640658</v>
+        <v>143.923765948135</v>
       </c>
       <c r="I9" s="2" t="n">
-        <v>6570.76</v>
+        <v>242371.99</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>1.7037792E12</v>
+        <v>1.703952E12</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>1.703865599999E12</v>
+        <v>1.704038399999E12</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>1.70382498E12</v>
+        <v>1.70399796E12</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>1.70385978E12</v>
+        <v>1.703964E12</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>146.25003814989213</v>
+        <v>138.48865502640658</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>147.20196967035423</v>
+        <v>140.63047373957855</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>137.2237751314403</v>
+        <v>137.5574753447999</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>139.7006888732879</v>
+        <v>139.7205451802579</v>
       </c>
       <c r="I10" s="2" t="n">
-        <v>30270.04</v>
+        <v>8432.36</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>1.7036928E12</v>
+        <v>1.7038656E12</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>1.703779199999E12</v>
+        <v>1.703951999999E12</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>1.70369742E12</v>
+        <v>1.7038692E12</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>1.70377278E12</v>
+        <v>1.70390106E12</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>147.7483564316613</v>
+        <v>139.7096543691948</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>154.9281042871005</v>
+        <v>140.1036556808429</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>146.25003814989213</v>
+        <v>137.2288543735375</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>146.25003814989213</v>
+        <v>138.48865502640658</v>
       </c>
       <c r="I11" s="2" t="n">
-        <v>17867.85</v>
+        <v>6570.76</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>1.7036064E12</v>
+        <v>1.7037792E12</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>1.703692799999E12</v>
+        <v>1.703865599999E12</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>1.70369052E12</v>
+        <v>1.70382498E12</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>1.70361936E12</v>
+        <v>1.70385978E12</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>132.61932011050416</v>
+        <v>146.25003814989213</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>148.20579687549966</v>
+        <v>147.20196967035423</v>
       </c>
       <c r="G12" s="2" t="n">
-        <v>131.1059391724075</v>
+        <v>137.2237751314403</v>
       </c>
       <c r="H12" s="2" t="n">
-        <v>147.79921898653836</v>
+        <v>139.7006888732879</v>
       </c>
       <c r="I12" s="2" t="n">
-        <v>32277.58</v>
+        <v>30270.04</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>1.70352E12</v>
+        <v>1.7036928E12</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>1.703606399999E12</v>
+        <v>1.703779199999E12</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>1.70352E12</v>
+        <v>1.70369742E12</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>1.70358378E12</v>
+        <v>1.70377278E12</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>137.0167008811185</v>
+        <v>147.7483564316613</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>137.0167008811185</v>
+        <v>154.9281042871005</v>
       </c>
       <c r="G13" s="2" t="n">
-        <v>129.69369141213002</v>
+        <v>146.25003814989213</v>
       </c>
       <c r="H13" s="2" t="n">
-        <v>132.61179959485955</v>
+        <v>146.25003814989213</v>
       </c>
       <c r="I13" s="2" t="n">
-        <v>17050.16</v>
+        <v>17867.85</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>1.7034336E12</v>
+        <v>1.7036064E12</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>1.703519999999E12</v>
+        <v>1.703692799999E12</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>1.7034807E12</v>
+        <v>1.70369052E12</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>1.703508E12</v>
+        <v>1.70361936E12</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>137.0355294849046</v>
+        <v>132.61932011050416</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>139.0791950886372</v>
+        <v>148.20579687549966</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>136.15373227492327</v>
+        <v>131.1059391724075</v>
       </c>
       <c r="H14" s="2" t="n">
-        <v>137.006778539165</v>
+        <v>147.79921898653836</v>
       </c>
       <c r="I14" s="2" t="n">
-        <v>44205.39</v>
+        <v>32277.58</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>1.7033472E12</v>
+        <v>1.70352E12</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>1.703433599999E12</v>
+        <v>1.703606399999E12</v>
       </c>
       <c r="C15" s="2" t="n">
-        <v>1.70335626E12</v>
+        <v>1.70352E12</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>1.70342952E12</v>
+        <v>1.70358378E12</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>141.69071751729788</v>
+        <v>137.0167008811185</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>142.7124969944635</v>
+        <v>137.0167008811185</v>
       </c>
       <c r="G15" s="2" t="n">
-        <v>135.21021362591745</v>
+        <v>129.69369141213002</v>
       </c>
       <c r="H15" s="2" t="n">
-        <v>137.0830509116974</v>
+        <v>132.61179959485955</v>
       </c>
       <c r="I15" s="2" t="n">
-        <v>42733.92</v>
+        <v>17050.16</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>1.7032608E12</v>
+        <v>1.7034336E12</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>1.703347199999E12</v>
+        <v>1.703519999999E12</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>1.70326182E12</v>
+        <v>1.7034807E12</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>1.70327496E12</v>
+        <v>1.703508E12</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>144.40198646689396</v>
+        <v>137.0355294849046</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>144.64685890455752</v>
+        <v>139.0791950886372</v>
       </c>
       <c r="G16" s="2" t="n">
-        <v>137.36240704869448</v>
+        <v>136.15373227492327</v>
       </c>
       <c r="H16" s="2" t="n">
-        <v>141.72262943066883</v>
+        <v>137.006778539165</v>
       </c>
       <c r="I16" s="2" t="n">
-        <v>59643.2</v>
+        <v>44205.39</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>1.7031744E12</v>
+        <v>1.7033472E12</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>1.703260799999E12</v>
+        <v>1.703433599999E12</v>
       </c>
       <c r="C17" s="2" t="n">
-        <v>1.70322852E12</v>
+        <v>1.70335626E12</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>1.70317554E12</v>
+        <v>1.70342952E12</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>131.50513821444477</v>
+        <v>141.69071751729788</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>147.69609700776292</v>
+        <v>142.7124969944635</v>
       </c>
       <c r="G17" s="2" t="n">
-        <v>131.25018382070522</v>
+        <v>135.21021362591745</v>
       </c>
       <c r="H17" s="2" t="n">
-        <v>144.41365662910698</v>
+        <v>137.0830509116974</v>
       </c>
       <c r="I17" s="2" t="n">
-        <v>686013.64</v>
+        <v>42733.92</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>1.703088E12</v>
+        <v>1.7032608E12</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>1.703174399999E12</v>
+        <v>1.703347199999E12</v>
       </c>
       <c r="C18" s="2" t="n">
-        <v>1.70313264E12</v>
+        <v>1.70326182E12</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>1.7030925E12</v>
+        <v>1.70327496E12</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>125.47437152442438</v>
+        <v>144.40198646689396</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>134.42729962263172</v>
+        <v>144.64685890455752</v>
       </c>
       <c r="G18" s="2" t="n">
-        <v>124.72694512955147</v>
+        <v>137.36240704869448</v>
       </c>
       <c r="H18" s="2" t="n">
-        <v>131.48430594274149</v>
+        <v>141.72262943066883</v>
       </c>
       <c r="I18" s="2" t="n">
-        <v>33765.81</v>
+        <v>59643.2</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>1.7030016E12</v>
+        <v>1.7031744E12</v>
       </c>
       <c r="B19" s="2" t="n">
-        <v>1.703087999999E12</v>
+        <v>1.703260799999E12</v>
       </c>
       <c r="C19" s="2" t="n">
-        <v>1.70305422E12</v>
+        <v>1.70322852E12</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>1.7030742E12</v>
+        <v>1.70317554E12</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>123.80012846254355</v>
+        <v>131.50513821444477</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>133.63659873839893</v>
+        <v>147.69609700776292</v>
       </c>
       <c r="G19" s="2" t="n">
-        <v>122.85206337941135</v>
+        <v>131.25018382070522</v>
       </c>
       <c r="H19" s="2" t="n">
-        <v>125.37542020785284</v>
+        <v>144.41365662910698</v>
       </c>
       <c r="I19" s="2" t="n">
-        <v>41021.56</v>
+        <v>686013.64</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>1.7029152E12</v>
+        <v>1.703088E12</v>
       </c>
       <c r="B20" s="2" t="n">
-        <v>1.703001599999E12</v>
+        <v>1.703174399999E12</v>
       </c>
       <c r="C20" s="2" t="n">
-        <v>1.70294526E12</v>
+        <v>1.70313264E12</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>1.70298018E12</v>
+        <v>1.7030925E12</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>128.98248199353392</v>
+        <v>125.47437152442438</v>
       </c>
       <c r="F20" s="2" t="n">
-        <v>133.05113865406884</v>
+        <v>134.42729962263172</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>122.04388369955518</v>
+        <v>124.72694512955147</v>
       </c>
       <c r="H20" s="2" t="n">
-        <v>123.80579753933254</v>
+        <v>131.48430594274149</v>
       </c>
       <c r="I20" s="2" t="n">
-        <v>59549.14</v>
+        <v>33765.81</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>1.7028288E12</v>
+        <v>1.7030016E12</v>
       </c>
       <c r="B21" s="2" t="n">
-        <v>1.702915199999E12</v>
+        <v>1.703087999999E12</v>
       </c>
       <c r="C21" s="2" t="n">
-        <v>1.70283096E12</v>
+        <v>1.70305422E12</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>1.70286702E12</v>
+        <v>1.7030742E12</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>131.67945241422743</v>
+        <v>123.80012846254355</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>131.80672104108498</v>
+        <v>133.63659873839893</v>
       </c>
       <c r="G21" s="2" t="n">
-        <v>123.46842371711385</v>
+        <v>122.85206337941135</v>
       </c>
       <c r="H21" s="2" t="n">
-        <v>129.00609560294623</v>
+        <v>125.37542020785284</v>
       </c>
       <c r="I21" s="2" t="n">
-        <v>55965.83</v>
+        <v>41021.56</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>1.7027424E12</v>
+        <v>1.7029152E12</v>
       </c>
       <c r="B22" s="2" t="n">
-        <v>1.702828799999E12</v>
+        <v>1.703001599999E12</v>
       </c>
       <c r="C22" s="2" t="n">
-        <v>1.70280606E12</v>
+        <v>1.70294526E12</v>
       </c>
       <c r="D22" s="2" t="n">
-        <v>1.70282826E12</v>
+        <v>1.70298018E12</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>136.02128297045758</v>
+        <v>128.98248199353392</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>136.95323074641684</v>
+        <v>133.05113865406884</v>
       </c>
       <c r="G22" s="2" t="n">
-        <v>131.54173224593924</v>
+        <v>122.04388369955518</v>
       </c>
       <c r="H22" s="2" t="n">
-        <v>131.67163693169798</v>
+        <v>123.80579753933254</v>
       </c>
       <c r="I22" s="2" t="n">
-        <v>36225.72</v>
+        <v>59549.14</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>1.702656E12</v>
+        <v>1.7028288E12</v>
       </c>
       <c r="B23" s="2" t="n">
-        <v>1.702742399999E12</v>
+        <v>1.702915199999E12</v>
       </c>
       <c r="C23" s="2" t="n">
-        <v>1.70271642E12</v>
+        <v>1.70283096E12</v>
       </c>
       <c r="D23" s="2" t="n">
-        <v>1.70265942E12</v>
+        <v>1.70286702E12</v>
       </c>
       <c r="E23" s="2" t="n">
-        <v>135.17524731079843</v>
+        <v>131.67945241422743</v>
       </c>
       <c r="F23" s="2" t="n">
-        <v>138.24733528840574</v>
+        <v>131.80672104108498</v>
       </c>
       <c r="G23" s="2" t="n">
-        <v>134.58275038689536</v>
+        <v>123.46842371711385</v>
       </c>
       <c r="H23" s="2" t="n">
-        <v>135.95307793024207</v>
+        <v>129.00609560294623</v>
       </c>
       <c r="I23" s="2" t="n">
-        <v>12915.12</v>
+        <v>55965.83</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>1.7025696E12</v>
+        <v>1.7027424E12</v>
       </c>
       <c r="B24" s="2" t="n">
-        <v>1.702655999999E12</v>
+        <v>1.702828799999E12</v>
       </c>
       <c r="C24" s="2" t="n">
-        <v>1.70256966E12</v>
+        <v>1.70280606E12</v>
       </c>
       <c r="D24" s="2" t="n">
-        <v>1.70265426E12</v>
+        <v>1.70282826E12</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>142.187683504841</v>
+        <v>136.02128297045758</v>
       </c>
       <c r="F24" s="2" t="n">
-        <v>142.21043220948695</v>
+        <v>136.95323074641684</v>
       </c>
       <c r="G24" s="2" t="n">
-        <v>135.0215734039484</v>
+        <v>131.54173224593924</v>
       </c>
       <c r="H24" s="2" t="n">
-        <v>135.18890398503666</v>
+        <v>131.67163693169798</v>
       </c>
       <c r="I24" s="2" t="n">
-        <v>3976.44</v>
+        <v>36225.72</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>1.7024832E12</v>
+        <v>1.702656E12</v>
       </c>
       <c r="B25" s="2" t="n">
-        <v>1.702569599999E12</v>
+        <v>1.702742399999E12</v>
       </c>
       <c r="C25" s="2" t="n">
-        <v>1.70256792E12</v>
+        <v>1.70271642E12</v>
       </c>
       <c r="D25" s="2" t="n">
-        <v>1.70253198E12</v>
+        <v>1.70265942E12</v>
       </c>
       <c r="E25" s="2" t="n">
-        <v>136.21450630933995</v>
+        <v>135.17524731079843</v>
       </c>
       <c r="F25" s="2" t="n">
-        <v>142.7267852786753</v>
+        <v>138.24733528840574</v>
       </c>
       <c r="G25" s="2" t="n">
-        <v>135.02848068997272</v>
+        <v>134.58275038689536</v>
       </c>
       <c r="H25" s="2" t="n">
-        <v>142.1617649093843</v>
+        <v>135.95307793024207</v>
       </c>
       <c r="I25" s="2" t="n">
-        <v>115548.53</v>
+        <v>12915.12</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>1.7023968E12</v>
+        <v>1.7025696E12</v>
       </c>
       <c r="B26" s="2" t="n">
-        <v>1.702483199999E12</v>
+        <v>1.702655999999E12</v>
       </c>
       <c r="C26" s="2" t="n">
-        <v>1.70247708E12</v>
+        <v>1.70256966E12</v>
       </c>
       <c r="D26" s="2" t="n">
-        <v>1.70241252E12</v>
+        <v>1.70265426E12</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>131.11140867183377</v>
+        <v>142.187683504841</v>
       </c>
       <c r="F26" s="2" t="n">
-        <v>137.40601135948586</v>
+        <v>142.21043220948695</v>
       </c>
       <c r="G26" s="2" t="n">
-        <v>126.52962293477927</v>
+        <v>135.0215734039484</v>
       </c>
       <c r="H26" s="2" t="n">
-        <v>136.2208966709233</v>
+        <v>135.18890398503666</v>
       </c>
       <c r="I26" s="2" t="n">
-        <v>37295.93</v>
+        <v>3976.44</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>1.7023104E12</v>
+        <v>1.7024832E12</v>
       </c>
       <c r="B27" s="2" t="n">
-        <v>1.702396799999E12</v>
+        <v>1.702569599999E12</v>
       </c>
       <c r="C27" s="2" t="n">
-        <v>1.70231886E12</v>
+        <v>1.70256792E12</v>
       </c>
       <c r="D27" s="2" t="n">
-        <v>1.7023893E12</v>
+        <v>1.70253198E12</v>
       </c>
       <c r="E27" s="2" t="n">
-        <v>131.92174831841749</v>
+        <v>136.21450630933995</v>
       </c>
       <c r="F27" s="2" t="n">
-        <v>132.99065888166157</v>
+        <v>142.7267852786753</v>
       </c>
       <c r="G27" s="2" t="n">
-        <v>127.5594065210483</v>
+        <v>135.02848068997272</v>
       </c>
       <c r="H27" s="2" t="n">
-        <v>131.12445834450864</v>
+        <v>142.1617649093843</v>
       </c>
       <c r="I27" s="2" t="n">
-        <v>28898.18</v>
+        <v>115548.53</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>1.702224E12</v>
+        <v>1.7023968E12</v>
       </c>
       <c r="B28" s="2" t="n">
-        <v>1.702310399999E12</v>
+        <v>1.702483199999E12</v>
       </c>
       <c r="C28" s="2" t="n">
-        <v>1.70222466E12</v>
+        <v>1.70247708E12</v>
       </c>
       <c r="D28" s="2" t="n">
-        <v>1.70229498E12</v>
+        <v>1.70241252E12</v>
       </c>
       <c r="E28" s="2" t="n">
-        <v>149.892397494413</v>
+        <v>131.11140867183377</v>
       </c>
       <c r="F28" s="2" t="n">
-        <v>150.0234567081854</v>
+        <v>137.40601135948586</v>
       </c>
       <c r="G28" s="2" t="n">
-        <v>127.72146056714688</v>
+        <v>126.52962293477927</v>
       </c>
       <c r="H28" s="2" t="n">
-        <v>131.93356007328487</v>
+        <v>136.2208966709233</v>
       </c>
       <c r="I28" s="2" t="n">
-        <v>284564.71</v>
+        <v>37295.93</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>1.7021376E12</v>
+        <v>1.7023104E12</v>
       </c>
       <c r="B29" s="2" t="n">
-        <v>1.702223999999E12</v>
+        <v>1.702396799999E12</v>
       </c>
       <c r="C29" s="2" t="n">
-        <v>1.70218878E12</v>
+        <v>1.70231886E12</v>
       </c>
       <c r="D29" s="2" t="n">
-        <v>1.70220864E12</v>
+        <v>1.7023893E12</v>
       </c>
       <c r="E29" s="2" t="n">
-        <v>147.95320958702064</v>
+        <v>131.92174831841749</v>
       </c>
       <c r="F29" s="2" t="n">
-        <v>153.90843651624505</v>
+        <v>132.99065888166157</v>
       </c>
       <c r="G29" s="2" t="n">
-        <v>145.63946711985267</v>
+        <v>127.5594065210483</v>
       </c>
       <c r="H29" s="2" t="n">
-        <v>149.88561724302386</v>
+        <v>131.12445834450864</v>
       </c>
       <c r="I29" s="2" t="n">
-        <v>159686.31</v>
+        <v>28898.18</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>1.7020512E12</v>
+        <v>1.702224E12</v>
       </c>
       <c r="B30" s="2" t="n">
-        <v>1.702137599999E12</v>
+        <v>1.702310399999E12</v>
       </c>
       <c r="C30" s="2" t="n">
-        <v>1.70208174E12</v>
+        <v>1.70222466E12</v>
       </c>
       <c r="D30" s="2" t="n">
-        <v>1.70213622E12</v>
+        <v>1.70229498E12</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>148.8558245466771</v>
+        <v>149.892397494413</v>
       </c>
       <c r="F30" s="2" t="n">
-        <v>152.37633118910318</v>
+        <v>150.0234567081854</v>
       </c>
       <c r="G30" s="2" t="n">
-        <v>147.6097158164336</v>
+        <v>127.72146056714688</v>
       </c>
       <c r="H30" s="2" t="n">
-        <v>147.95037325229387</v>
+        <v>131.93356007328487</v>
       </c>
       <c r="I30" s="2" t="n">
-        <v>9119.63</v>
+        <v>284564.71</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>1.7019648E12</v>
+        <v>1.7021376E12</v>
       </c>
       <c r="B31" s="2" t="n">
-        <v>1.702051199999E12</v>
+        <v>1.702223999999E12</v>
       </c>
       <c r="C31" s="2" t="n">
-        <v>1.70198046E12</v>
+        <v>1.70218878E12</v>
       </c>
       <c r="D31" s="2" t="n">
-        <v>1.7020008E12</v>
+        <v>1.70220864E12</v>
       </c>
       <c r="E31" s="2" t="n">
-        <v>148.26011677988598</v>
+        <v>147.95320958702064</v>
       </c>
       <c r="F31" s="2" t="n">
-        <v>152.52877462465156</v>
+        <v>153.90843651624505</v>
       </c>
       <c r="G31" s="2" t="n">
-        <v>147.63839818660435</v>
+        <v>145.63946711985267</v>
       </c>
       <c r="H31" s="2" t="n">
-        <v>148.85891717143443</v>
+        <v>149.88561724302386</v>
       </c>
       <c r="I31" s="2" t="n">
-        <v>49817.05</v>
+        <v>159686.31</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>1.7018784E12</v>
+        <v>1.7020512E12</v>
       </c>
       <c r="B32" s="2" t="n">
-        <v>1.701964799999E12</v>
+        <v>1.702137599999E12</v>
       </c>
       <c r="C32" s="2" t="n">
-        <v>1.70195616E12</v>
+        <v>1.70208174E12</v>
       </c>
       <c r="D32" s="2" t="n">
-        <v>1.70191254E12</v>
+        <v>1.70213622E12</v>
       </c>
       <c r="E32" s="2" t="n">
-        <v>133.4094267767442</v>
+        <v>148.8558245466771</v>
       </c>
       <c r="F32" s="2" t="n">
-        <v>149.5517032654528</v>
+        <v>152.37633118910318</v>
       </c>
       <c r="G32" s="2" t="n">
-        <v>133.26266453838545</v>
+        <v>147.6097158164336</v>
       </c>
       <c r="H32" s="2" t="n">
-        <v>148.25613917537143</v>
+        <v>147.95037325229387</v>
       </c>
       <c r="I32" s="2" t="n">
-        <v>82805.55</v>
+        <v>9119.63</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>1.701792E12</v>
+        <v>1.7019648E12</v>
       </c>
       <c r="B33" s="2" t="n">
-        <v>1.701878399999E12</v>
+        <v>1.702051199999E12</v>
       </c>
       <c r="C33" s="2" t="n">
-        <v>1.70179602E12</v>
+        <v>1.70198046E12</v>
       </c>
       <c r="D33" s="2" t="n">
-        <v>1.70187834E12</v>
+        <v>1.7020008E12</v>
       </c>
       <c r="E33" s="2" t="n">
-        <v>141.67841496823283</v>
+        <v>148.26011677988598</v>
       </c>
       <c r="F33" s="2" t="n">
-        <v>142.61842862257743</v>
+        <v>152.52877462465156</v>
       </c>
       <c r="G33" s="2" t="n">
-        <v>133.42417721884414</v>
+        <v>147.63839818660435</v>
       </c>
       <c r="H33" s="2" t="n">
-        <v>133.42417721884414</v>
+        <v>148.85891717143443</v>
       </c>
       <c r="I33" s="2" t="n">
-        <v>23308.1</v>
+        <v>49817.05</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>1.7017056E12</v>
+        <v>1.7018784E12</v>
       </c>
       <c r="B34" s="2" t="n">
-        <v>1.701791999999E12</v>
+        <v>1.701964799999E12</v>
       </c>
       <c r="C34" s="2" t="n">
-        <v>1.70177316E12</v>
+        <v>1.70195616E12</v>
       </c>
       <c r="D34" s="2" t="n">
-        <v>1.7017563E12</v>
+        <v>1.70191254E12</v>
       </c>
       <c r="E34" s="2" t="n">
-        <v>135.3020149700363</v>
+        <v>133.4094267767442</v>
       </c>
       <c r="F34" s="2" t="n">
-        <v>143.4163917061905</v>
+        <v>149.5517032654528</v>
       </c>
       <c r="G34" s="2" t="n">
-        <v>131.75976366845126</v>
+        <v>133.26266453838545</v>
       </c>
       <c r="H34" s="2" t="n">
-        <v>141.71578247964356</v>
+        <v>148.25613917537143</v>
       </c>
       <c r="I34" s="2" t="n">
-        <v>54934.12</v>
+        <v>82805.55</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>1.7016192E12</v>
+        <v>1.701792E12</v>
       </c>
       <c r="B35" s="2" t="n">
-        <v>1.701705599999E12</v>
+        <v>1.701878399999E12</v>
       </c>
       <c r="C35" s="2" t="n">
-        <v>1.70165832E12</v>
+        <v>1.70179602E12</v>
       </c>
       <c r="D35" s="2" t="n">
-        <v>1.7016192E12</v>
+        <v>1.70187834E12</v>
       </c>
       <c r="E35" s="2" t="n">
-        <v>129.63076145151805</v>
+        <v>141.67841496823283</v>
       </c>
       <c r="F35" s="2" t="n">
-        <v>138.01550123691547</v>
+        <v>142.61842862257743</v>
       </c>
       <c r="G35" s="2" t="n">
-        <v>129.63076145151805</v>
+        <v>133.42417721884414</v>
       </c>
       <c r="H35" s="2" t="n">
-        <v>135.2857432636967</v>
+        <v>133.42417721884414</v>
       </c>
       <c r="I35" s="2" t="n">
-        <v>58857.27</v>
+        <v>23308.1</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>1.7015328E12</v>
+        <v>1.7017056E12</v>
       </c>
       <c r="B36" s="2" t="n">
-        <v>1.701619199999E12</v>
+        <v>1.701791999999E12</v>
       </c>
       <c r="C36" s="2" t="n">
-        <v>1.70161338E12</v>
+        <v>1.70177316E12</v>
       </c>
       <c r="D36" s="2" t="n">
-        <v>1.70158854E12</v>
+        <v>1.7017563E12</v>
       </c>
       <c r="E36" s="2" t="n">
-        <v>126.19531482684356</v>
+        <v>135.3020149700363</v>
       </c>
       <c r="F36" s="2" t="n">
-        <v>131.56593260067103</v>
+        <v>143.4163917061905</v>
       </c>
       <c r="G36" s="2" t="n">
-        <v>125.42576394002714</v>
+        <v>131.75976366845126</v>
       </c>
       <c r="H36" s="2" t="n">
-        <v>129.5294593901089</v>
+        <v>141.71578247964356</v>
       </c>
       <c r="I36" s="2" t="n">
-        <v>121530.62</v>
+        <v>54934.12</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>1.7014464E12</v>
+        <v>1.7016192E12</v>
       </c>
       <c r="B37" s="2" t="n">
-        <v>1.701532799999E12</v>
+        <v>1.701705599999E12</v>
       </c>
       <c r="C37" s="2" t="n">
-        <v>1.70151552E12</v>
+        <v>1.70165832E12</v>
       </c>
       <c r="D37" s="2" t="n">
-        <v>1.70144646E12</v>
+        <v>1.7016192E12</v>
       </c>
       <c r="E37" s="2" t="n">
-        <v>117.29475538474315</v>
+        <v>129.63076145151805</v>
       </c>
       <c r="F37" s="2" t="n">
-        <v>126.69819507649068</v>
+        <v>138.01550123691547</v>
       </c>
       <c r="G37" s="2" t="n">
-        <v>117.28257310366843</v>
+        <v>129.63076145151805</v>
       </c>
       <c r="H37" s="2" t="n">
-        <v>126.18626511089035</v>
+        <v>135.2857432636967</v>
       </c>
       <c r="I37" s="2" t="n">
-        <v>105574.14</v>
+        <v>58857.27</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>1.70136E12</v>
+        <v>1.7015328E12</v>
       </c>
       <c r="B38" s="2" t="n">
-        <v>1.701446399999E12</v>
+        <v>1.701619199999E12</v>
       </c>
       <c r="C38" s="2" t="n">
-        <v>1.70139366E12</v>
+        <v>1.70161338E12</v>
       </c>
       <c r="D38" s="2" t="n">
-        <v>1.70136198E12</v>
+        <v>1.70158854E12</v>
       </c>
       <c r="E38" s="2" t="n">
-        <v>113.06122264088386</v>
+        <v>126.19531482684356</v>
       </c>
       <c r="F38" s="2" t="n">
-        <v>118.72414146971165</v>
+        <v>131.56593260067103</v>
       </c>
       <c r="G38" s="2" t="n">
-        <v>112.78004672062687</v>
+        <v>125.42576394002714</v>
       </c>
       <c r="H38" s="2" t="n">
-        <v>117.29851355512</v>
+        <v>129.5294593901089</v>
       </c>
       <c r="I38" s="2" t="n">
-        <v>23764.8</v>
+        <v>121530.62</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>1.7012736E12</v>
+        <v>1.7014464E12</v>
       </c>
       <c r="B39" s="2" t="n">
-        <v>1.701359999999E12</v>
+        <v>1.701532799999E12</v>
       </c>
       <c r="C39" s="2" t="n">
-        <v>1.70128914E12</v>
+        <v>1.70151552E12</v>
       </c>
       <c r="D39" s="2" t="n">
-        <v>1.70132694E12</v>
+        <v>1.70144646E12</v>
       </c>
       <c r="E39" s="2" t="n">
-        <v>112.40147177148806</v>
+        <v>117.29475538474315</v>
       </c>
       <c r="F39" s="2" t="n">
-        <v>113.15561040799287</v>
+        <v>126.69819507649068</v>
       </c>
       <c r="G39" s="2" t="n">
-        <v>111.43276399182467</v>
+        <v>117.28257310366843</v>
       </c>
       <c r="H39" s="2" t="n">
-        <v>113.06767804974085</v>
+        <v>126.18626511089035</v>
       </c>
       <c r="I39" s="2" t="n">
-        <v>2622.08</v>
+        <v>105574.14</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>1.7011872E12</v>
+        <v>1.70136E12</v>
       </c>
       <c r="B40" s="2" t="n">
-        <v>1.701273599999E12</v>
+        <v>1.701446399999E12</v>
       </c>
       <c r="C40" s="2" t="n">
-        <v>1.7012196E12</v>
+        <v>1.70139366E12</v>
       </c>
       <c r="D40" s="2" t="n">
-        <v>1.70124714E12</v>
+        <v>1.70136198E12</v>
       </c>
       <c r="E40" s="2" t="n">
-        <v>113.74722759570152</v>
+        <v>113.06122264088386</v>
       </c>
       <c r="F40" s="2" t="n">
-        <v>115.30094269021346</v>
+        <v>118.72414146971165</v>
       </c>
       <c r="G40" s="2" t="n">
-        <v>111.98030418287038</v>
+        <v>112.78004672062687</v>
       </c>
       <c r="H40" s="2" t="n">
-        <v>112.39105956150648</v>
+        <v>117.29851355512</v>
       </c>
       <c r="I40" s="2" t="n">
-        <v>11034.63</v>
+        <v>23764.8</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>1.7011008E12</v>
+        <v>1.7012736E12</v>
       </c>
       <c r="B41" s="2" t="n">
-        <v>1.701187199999E12</v>
+        <v>1.701359999999E12</v>
       </c>
       <c r="C41" s="2" t="n">
-        <v>1.70116464E12</v>
+        <v>1.70128914E12</v>
       </c>
       <c r="D41" s="2" t="n">
-        <v>1.70112294E12</v>
+        <v>1.70132694E12</v>
       </c>
       <c r="E41" s="2" t="n">
-        <v>110.42154460049468</v>
+        <v>112.40147177148806</v>
       </c>
       <c r="F41" s="2" t="n">
-        <v>115.17297070319817</v>
+        <v>113.15561040799287</v>
       </c>
       <c r="G41" s="2" t="n">
-        <v>108.96959848863276</v>
+        <v>111.43276399182467</v>
       </c>
       <c r="H41" s="2" t="n">
-        <v>113.79050986570684</v>
+        <v>113.06767804974085</v>
       </c>
       <c r="I41" s="2" t="n">
-        <v>46216.1</v>
+        <v>2622.08</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
+        <v>1.7011872E12</v>
+      </c>
+      <c r="B42" s="2" t="n">
+        <v>1.701273599999E12</v>
+      </c>
+      <c r="C42" s="2" t="n">
+        <v>1.7012196E12</v>
+      </c>
+      <c r="D42" s="2" t="n">
+        <v>1.70124714E12</v>
+      </c>
+      <c r="E42" s="2" t="n">
+        <v>113.74722759570152</v>
+      </c>
+      <c r="F42" s="2" t="n">
+        <v>115.30094269021346</v>
+      </c>
+      <c r="G42" s="2" t="n">
+        <v>111.98030418287038</v>
+      </c>
+      <c r="H42" s="2" t="n">
+        <v>112.39105956150648</v>
+      </c>
+      <c r="I42" s="2" t="n">
+        <v>11034.63</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="2" t="n">
+        <v>1.7011008E12</v>
+      </c>
+      <c r="B43" s="2" t="n">
+        <v>1.701187199999E12</v>
+      </c>
+      <c r="C43" s="2" t="n">
+        <v>1.70116464E12</v>
+      </c>
+      <c r="D43" s="2" t="n">
+        <v>1.70112294E12</v>
+      </c>
+      <c r="E43" s="2" t="n">
+        <v>110.42154460049468</v>
+      </c>
+      <c r="F43" s="2" t="n">
+        <v>115.17297070319817</v>
+      </c>
+      <c r="G43" s="2" t="n">
+        <v>108.96959848863276</v>
+      </c>
+      <c r="H43" s="2" t="n">
+        <v>113.79050986570684</v>
+      </c>
+      <c r="I43" s="2" t="n">
+        <v>46216.1</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="n">
         <v>1.7010144E12</v>
       </c>
-      <c r="B42" s="2" t="n">
+      <c r="B44" s="2" t="n">
         <v>1.701100799999E12</v>
       </c>
-      <c r="C42" s="2" t="n">
+      <c r="C44" s="2" t="n">
         <v>1.70101866E12</v>
       </c>
-      <c r="D42" s="2" t="n">
+      <c r="D44" s="2" t="n">
         <v>1.7010858E12</v>
       </c>
-      <c r="E42" s="2" t="n">
+      <c r="E44" s="2" t="n">
         <v>116.57122926365027</v>
       </c>
-      <c r="F42" s="2" t="n">
+      <c r="F44" s="2" t="n">
         <v>116.85701901988709</v>
       </c>
-      <c r="G42" s="2" t="n">
+      <c r="G44" s="2" t="n">
         <v>108.27048757442994</v>
       </c>
-      <c r="H42" s="2" t="n">
+      <c r="H44" s="2" t="n">
         <v>110.42687357282114</v>
       </c>
-      <c r="I42" s="2" t="n">
+      <c r="I44" s="2" t="n">
         <v>88802.54</v>
       </c>
     </row>

</xml_diff>